<commit_message>
a model simulate nuclear wind farm performance and economic with four months grid data
</commit_message>
<xml_diff>
--- a/example/hybrid_model/system_lifetime_performance.xlsx
+++ b/example/hybrid_model/system_lifetime_performance.xlsx
@@ -561,16 +561,16 @@
         <v>72</v>
       </c>
       <c r="G5" s="3">
-        <v>441099.0122222222</v>
+        <v>459596.8893580333</v>
       </c>
       <c r="H5" s="3">
-        <v>104183.5865909149</v>
+        <v>87440.32838484559</v>
       </c>
       <c r="I5" s="3">
         <v>0</v>
       </c>
       <c r="J5" s="3">
-        <v>39105.18644412385</v>
+        <v>32376.06915003818</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -593,16 +593,16 @@
         <v>72</v>
       </c>
       <c r="G6" s="3">
-        <v>441099.0122222222</v>
+        <v>459596.8893580333</v>
       </c>
       <c r="H6" s="3">
-        <v>104183.5865909149</v>
+        <v>87440.32838484559</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>39105.18644412385</v>
+        <v>32376.06915003818</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -625,16 +625,16 @@
         <v>144</v>
       </c>
       <c r="G7" s="3">
-        <v>882198.0244444445</v>
+        <v>919193.7787160666</v>
       </c>
       <c r="H7" s="3">
-        <v>204477.7367481358</v>
+        <v>175939.9156559471</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>79657.66429882475</v>
+        <v>65281.23913692087</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -657,16 +657,16 @@
         <v>144</v>
       </c>
       <c r="G8" s="3">
-        <v>882198.0244444445</v>
+        <v>919193.7787160666</v>
       </c>
       <c r="H8" s="3">
-        <v>204477.7367481358</v>
+        <v>175939.9156559471</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>79657.66429882475</v>
+        <v>65281.23913692087</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -689,16 +689,16 @@
         <v>216</v>
       </c>
       <c r="G9" s="3">
-        <v>1323297.036666667</v>
+        <v>1378790.6680741</v>
       </c>
       <c r="H9" s="3">
-        <v>337215.0017243707</v>
+        <v>265499.7793553168</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>127918.1091135462</v>
+        <v>98567.32161440127</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -721,16 +721,16 @@
         <v>216</v>
       </c>
       <c r="G10" s="3">
-        <v>1323297.036666667</v>
+        <v>1378790.6680741</v>
       </c>
       <c r="H10" s="3">
-        <v>337215.0017243707</v>
+        <v>265499.7793553168</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>127918.1091135462</v>
+        <v>98567.32161440127</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -753,16 +753,16 @@
         <v>288</v>
       </c>
       <c r="G11" s="3">
-        <v>1764396.048888889</v>
+        <v>1838387.557432133</v>
       </c>
       <c r="H11" s="3">
-        <v>443156.2923597118</v>
+        <v>351604.8140642748</v>
       </c>
       <c r="I11" s="3">
-        <v>0</v>
+        <v>0.873350509689706</v>
       </c>
       <c r="J11" s="3">
-        <v>169650.6335541952</v>
+        <v>130857.7343420096</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -785,16 +785,16 @@
         <v>288</v>
       </c>
       <c r="G12" s="3">
-        <v>1764396.048888889</v>
+        <v>1838387.557432133</v>
       </c>
       <c r="H12" s="3">
-        <v>443156.2923597118</v>
+        <v>351604.8140642748</v>
       </c>
       <c r="I12" s="3">
-        <v>0</v>
+        <v>0.873350509689706</v>
       </c>
       <c r="J12" s="3">
-        <v>169650.6335541952</v>
+        <v>130857.7343420096</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -817,16 +817,16 @@
         <v>360</v>
       </c>
       <c r="G13" s="3">
-        <v>2205495.061111113</v>
+        <v>2297984.446790164</v>
       </c>
       <c r="H13" s="3">
-        <v>501290.5036987989</v>
+        <v>444388.4130639153</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>190725.2592114788</v>
+        <v>165013.6639672196</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -849,16 +849,16 @@
         <v>360</v>
       </c>
       <c r="G14" s="3">
-        <v>2205495.061111113</v>
+        <v>2297984.446790164</v>
       </c>
       <c r="H14" s="3">
-        <v>501290.5036987989</v>
+        <v>444388.4130639153</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <v>190725.2592114788</v>
+        <v>165013.6639672196</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -881,16 +881,16 @@
         <v>432</v>
       </c>
       <c r="G15" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H15" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I15" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J15" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -913,16 +913,16 @@
         <v>432</v>
       </c>
       <c r="G16" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H16" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I16" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J16" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -945,16 +945,16 @@
         <v>432</v>
       </c>
       <c r="G17" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H17" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I17" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J17" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -977,16 +977,16 @@
         <v>432</v>
       </c>
       <c r="G18" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H18" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I18" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J18" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1009,16 +1009,16 @@
         <v>432</v>
       </c>
       <c r="G19" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H19" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I19" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J19" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1041,16 +1041,16 @@
         <v>432</v>
       </c>
       <c r="G20" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H20" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I20" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J20" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1073,16 +1073,16 @@
         <v>432</v>
       </c>
       <c r="G21" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H21" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I21" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J21" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1105,16 +1105,16 @@
         <v>432</v>
       </c>
       <c r="G22" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H22" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I22" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J22" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1137,16 +1137,16 @@
         <v>432</v>
       </c>
       <c r="G23" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H23" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I23" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J23" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1169,16 +1169,16 @@
         <v>432</v>
       </c>
       <c r="G24" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H24" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I24" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J24" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1201,16 +1201,16 @@
         <v>432</v>
       </c>
       <c r="G25" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H25" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I25" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J25" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1233,16 +1233,16 @@
         <v>432</v>
       </c>
       <c r="G26" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H26" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I26" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J26" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1265,16 +1265,16 @@
         <v>432</v>
       </c>
       <c r="G27" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H27" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I27" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J27" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1297,16 +1297,16 @@
         <v>432</v>
       </c>
       <c r="G28" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H28" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I28" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J28" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1329,16 +1329,16 @@
         <v>432</v>
       </c>
       <c r="G29" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H29" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I29" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J29" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1361,16 +1361,16 @@
         <v>432</v>
       </c>
       <c r="G30" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H30" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I30" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J30" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1393,16 +1393,16 @@
         <v>432</v>
       </c>
       <c r="G31" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H31" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I31" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J31" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1425,16 +1425,16 @@
         <v>432</v>
       </c>
       <c r="G32" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H32" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I32" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J32" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1457,16 +1457,16 @@
         <v>432</v>
       </c>
       <c r="G33" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H33" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I33" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J33" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1489,16 +1489,16 @@
         <v>432</v>
       </c>
       <c r="G34" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H34" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J34" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1521,16 +1521,16 @@
         <v>432</v>
       </c>
       <c r="G35" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H35" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I35" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J35" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1553,16 +1553,16 @@
         <v>432</v>
       </c>
       <c r="G36" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H36" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I36" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J36" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1585,16 +1585,16 @@
         <v>432</v>
       </c>
       <c r="G37" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H37" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I37" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J37" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1617,16 +1617,16 @@
         <v>432</v>
       </c>
       <c r="G38" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H38" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I38" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J38" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1649,16 +1649,16 @@
         <v>432</v>
       </c>
       <c r="G39" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H39" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J39" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1681,16 +1681,16 @@
         <v>432</v>
       </c>
       <c r="G40" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H40" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I40" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J40" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1713,16 +1713,16 @@
         <v>432</v>
       </c>
       <c r="G41" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H41" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I41" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J41" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1745,16 +1745,16 @@
         <v>432</v>
       </c>
       <c r="G42" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H42" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I42" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J42" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1777,16 +1777,16 @@
         <v>432</v>
       </c>
       <c r="G43" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H43" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I43" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J43" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1809,16 +1809,16 @@
         <v>432</v>
       </c>
       <c r="G44" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H44" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I44" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J44" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1841,16 +1841,16 @@
         <v>432</v>
       </c>
       <c r="G45" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H45" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I45" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J45" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1873,16 +1873,16 @@
         <v>432</v>
       </c>
       <c r="G46" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H46" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I46" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J46" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1905,16 +1905,16 @@
         <v>432</v>
       </c>
       <c r="G47" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H47" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J47" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1937,16 +1937,16 @@
         <v>432</v>
       </c>
       <c r="G48" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H48" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I48" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J48" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -1969,16 +1969,16 @@
         <v>432</v>
       </c>
       <c r="G49" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H49" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I49" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J49" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2001,16 +2001,16 @@
         <v>432</v>
       </c>
       <c r="G50" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H50" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I50" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J50" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2033,16 +2033,16 @@
         <v>432</v>
       </c>
       <c r="G51" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H51" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I51" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J51" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2065,16 +2065,16 @@
         <v>432</v>
       </c>
       <c r="G52" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H52" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I52" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J52" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2097,16 +2097,16 @@
         <v>432</v>
       </c>
       <c r="G53" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H53" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I53" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J53" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2129,16 +2129,16 @@
         <v>432</v>
       </c>
       <c r="G54" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H54" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I54" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J54" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2161,16 +2161,16 @@
         <v>432</v>
       </c>
       <c r="G55" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H55" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I55" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J55" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2193,16 +2193,16 @@
         <v>432</v>
       </c>
       <c r="G56" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H56" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I56" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J56" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2225,16 +2225,16 @@
         <v>432</v>
       </c>
       <c r="G57" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H57" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I57" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J57" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2257,16 +2257,16 @@
         <v>432</v>
       </c>
       <c r="G58" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H58" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I58" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J58" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2289,16 +2289,16 @@
         <v>432</v>
       </c>
       <c r="G59" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H59" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I59" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J59" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2321,16 +2321,16 @@
         <v>432</v>
       </c>
       <c r="G60" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H60" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I60" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J60" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2353,16 +2353,16 @@
         <v>432</v>
       </c>
       <c r="G61" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H61" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I61" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J61" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2385,16 +2385,16 @@
         <v>432</v>
       </c>
       <c r="G62" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H62" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I62" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J62" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2417,16 +2417,16 @@
         <v>432</v>
       </c>
       <c r="G63" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H63" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I63" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J63" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2449,16 +2449,16 @@
         <v>432</v>
       </c>
       <c r="G64" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H64" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I64" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J64" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2481,16 +2481,16 @@
         <v>432</v>
       </c>
       <c r="G65" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H65" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I65" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J65" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2513,16 +2513,16 @@
         <v>432</v>
       </c>
       <c r="G66" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H66" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I66" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J66" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2545,16 +2545,16 @@
         <v>432</v>
       </c>
       <c r="G67" s="3">
-        <v>2646594.073333335</v>
+        <v>2757581.3361482</v>
       </c>
       <c r="H67" s="3">
-        <v>624150.9992613856</v>
+        <v>527519.8281481991</v>
       </c>
       <c r="I67" s="3">
-        <v>0</v>
+        <v>1.310025764534559</v>
       </c>
       <c r="J67" s="3">
-        <v>244986.1908102994</v>
+        <v>195382.086049675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>